<commit_message>
Add txt and improve inference to Excel + scraper
</commit_message>
<xml_diff>
--- a/Predictions.xlsx
+++ b/Predictions.xlsx
@@ -2,41 +2,26 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\OneDrive\Documents\Python\MMA Betting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770F99C0-FE2B-4AF9-9088-4E402A8E4531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD69E99E-2187-4E30-9C3F-291754A3CEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="14880" xr2:uid="{D89B7DE8-5654-4094-843D-B09E48B47E15}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New" sheetId="1" r:id="rId1"/>
+    <sheet name="Old" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="59">
   <si>
     <t>Fighter_1</t>
   </si>
@@ -44,49 +29,175 @@
     <t>Fighter_2</t>
   </si>
   <si>
-    <t>Jon Jones</t>
-  </si>
-  <si>
-    <t>Islam Makhachev</t>
-  </si>
-  <si>
-    <t>Justin Gaethje</t>
-  </si>
-  <si>
     <t>Weight</t>
   </si>
   <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Prob_1</t>
+  </si>
+  <si>
+    <t>Prob_2</t>
+  </si>
+  <si>
+    <t>MarQuel Mederos</t>
+  </si>
+  <si>
+    <t>Austin Hubbard</t>
+  </si>
+  <si>
     <t>Lw</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
-    <t>Tom Aspinall</t>
-  </si>
-  <si>
-    <t>Hw</t>
-  </si>
-  <si>
-    <t>Prob_1</t>
-  </si>
-  <si>
-    <t>Prob_2</t>
-  </si>
-  <si>
-    <t>Leon Edwards</t>
-  </si>
-  <si>
-    <t>Sean Brady</t>
-  </si>
-  <si>
-    <t>Ww</t>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>Jamall Emmers</t>
+  </si>
+  <si>
+    <t>Gabriel Miranda</t>
+  </si>
+  <si>
+    <t>Ft</t>
+  </si>
+  <si>
+    <t>0.06</t>
+  </si>
+  <si>
+    <t>0.94</t>
+  </si>
+  <si>
+    <t>Rafa Garcia</t>
+  </si>
+  <si>
+    <t>Vinc Pichel</t>
+  </si>
+  <si>
+    <t>0.36</t>
+  </si>
+  <si>
+    <t>0.64</t>
+  </si>
+  <si>
+    <t>Loopy Godinez</t>
+  </si>
+  <si>
+    <t>Julia Polastri</t>
+  </si>
+  <si>
+    <t>Ws</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>Christian Rodriguez</t>
+  </si>
+  <si>
+    <t>Melquizael Costa</t>
+  </si>
+  <si>
+    <t>0.62</t>
+  </si>
+  <si>
+    <t>0.38</t>
+  </si>
+  <si>
+    <t>Jose Daniel Medina</t>
+  </si>
+  <si>
+    <t>Ateba Gautier</t>
+  </si>
+  <si>
+    <t>Mw</t>
+  </si>
+  <si>
+    <t>Edgar Chairez</t>
+  </si>
+  <si>
+    <t>CJ Vergara</t>
+  </si>
+  <si>
+    <t>Fl</t>
+  </si>
+  <si>
+    <t>0.72</t>
+  </si>
+  <si>
+    <t>0.28</t>
+  </si>
+  <si>
+    <t>Ronaldo Rodriguez</t>
+  </si>
+  <si>
+    <t>Kevin Borjas</t>
+  </si>
+  <si>
+    <t>David Martinez</t>
+  </si>
+  <si>
+    <t>Saimon Oliveira</t>
+  </si>
+  <si>
+    <t>Bw</t>
+  </si>
+  <si>
+    <t>Raul Rosas Jr.</t>
+  </si>
+  <si>
+    <t>Vince Morales</t>
+  </si>
+  <si>
+    <t>0.32</t>
+  </si>
+  <si>
+    <t>0.68</t>
+  </si>
+  <si>
+    <t>Kelvin Gastelum</t>
+  </si>
+  <si>
+    <t>Joe Pyfer</t>
+  </si>
+  <si>
+    <t>0.52</t>
+  </si>
+  <si>
+    <t>0.48</t>
+  </si>
+  <si>
+    <t>Manuel Torres</t>
+  </si>
+  <si>
+    <t>Drew Dober</t>
+  </si>
+  <si>
+    <t>Brandon Moreno</t>
+  </si>
+  <si>
+    <t>Steve Erceg</t>
+  </si>
+  <si>
+    <t>0.66</t>
+  </si>
+  <si>
+    <t>0.34</t>
   </si>
 </sst>
 </file>
@@ -457,17 +568,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF18733C-2130-4485-8A7D-ABBE2ADC7A66}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="A1:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -478,70 +589,605 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66C6F167-FE00-4F1F-BC99-503D7CE92D77}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s">
         <v>9</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>